<commit_message>
scraped all posts urls
</commit_message>
<xml_diff>
--- a/scraped-data.xlsx
+++ b/scraped-data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="355">
   <si>
     <t>domain-name</t>
   </si>
@@ -259,6 +259,13 @@
   </si>
   <si>
     <t xml:space="preserve">
+    CHATEAU LES HAUTS D'AGLAN    </t>
+  </si>
+  <si>
+    <t>Isabelle REY AURIAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
     DOMAINE THOMAS-LABAILLE    </t>
   </si>
   <si>
@@ -290,13 +297,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-    CHATEAU LES HAUTS D'AGLAN    </t>
-  </si>
-  <si>
-    <t>Isabelle REY AURIAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
     CHATEAU LA BRETONNIERE    </t>
   </si>
   <si>
@@ -480,6 +480,654 @@
   </si>
   <si>
     <t>CHATEAU LA MARTINETTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DES AUMEDES    </t>
+  </si>
+  <si>
+    <t>Yves NORMAND</t>
+  </si>
+  <si>
+    <t>297, Chemin De Paille</t>
+  </si>
+  <si>
+    <t>04 94 73 70 32</t>
+  </si>
+  <si>
+    <t>DOMAINE DES AUMEDES Côtes de Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE DES AUMEDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DU HARRY    </t>
+  </si>
+  <si>
+    <t>Sauboires</t>
+  </si>
+  <si>
+    <t>32370</t>
+  </si>
+  <si>
+    <t>MANCIET</t>
+  </si>
+  <si>
+    <t>05 62 08 52 99</t>
+  </si>
+  <si>
+    <t>DOMAINE DU HARRY Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DU HARRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE D'EMBIDOURE    </t>
+  </si>
+  <si>
+    <t>Nathalie et Sandrine MENEGAZZO</t>
+  </si>
+  <si>
+    <t>Domaine Embidoure</t>
+  </si>
+  <si>
+    <t>32390</t>
+  </si>
+  <si>
+    <t>REJAUMONT</t>
+  </si>
+  <si>
+    <t>05 62 65 28 92</t>
+  </si>
+  <si>
+    <t>www.domaine-embidoure.com</t>
+  </si>
+  <si>
+    <t>DOMAINE D'EMBIDOURE Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE D'EMBIDOURE</t>
+  </si>
+  <si>
+    <t>Caractéristique : Moelleux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    LE BARTAT    </t>
+  </si>
+  <si>
+    <t>Pierre FITAN</t>
+  </si>
+  <si>
+    <t>32400</t>
+  </si>
+  <si>
+    <t>MAULICHERES</t>
+  </si>
+  <si>
+    <t>05 62 69 77 39</t>
+  </si>
+  <si>
+    <t>DOMAINE LE BARTAT Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE LE BARTAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    CHATEAU BARREJAT    </t>
+  </si>
+  <si>
+    <t>Denis CAPMARTIN</t>
+  </si>
+  <si>
+    <t>MAUMUSSON</t>
+  </si>
+  <si>
+    <t>05 62 69 74 92</t>
+  </si>
+  <si>
+    <t>CHATEAU BARREJAT Pacherenc du Vic-Bilh</t>
+  </si>
+  <si>
+    <t>A.O.C Pacherenc du Vic-Bilh</t>
+  </si>
+  <si>
+    <t>CHATEAU BARREJAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE LABRANCHE LAFFONT    </t>
+  </si>
+  <si>
+    <t>Christine DUPUY</t>
+  </si>
+  <si>
+    <t>05 62 69 74 90</t>
+  </si>
+  <si>
+    <t>DOMAINE LABRANCHE LAFFONT Pacherenc du Vic-Bilh</t>
+  </si>
+  <si>
+    <t>DOMAINE LABRANCHE LAFFONT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    LANGLA EMMANUELLE ET OLIVIER    </t>
+  </si>
+  <si>
+    <t>Olivier LANGLA</t>
+  </si>
+  <si>
+    <t>SARRAGACHIES</t>
+  </si>
+  <si>
+    <t>05 62 69 73 99</t>
+  </si>
+  <si>
+    <t>DOMAINE LAPRUNE Floc de Gascogne</t>
+  </si>
+  <si>
+    <t>A.O.C Floc de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE LAPRUNE</t>
+  </si>
+  <si>
+    <t>Type de produit : VDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    EARL DE BERNET    </t>
+  </si>
+  <si>
+    <t>Yves DOUSSAU</t>
+  </si>
+  <si>
+    <t>Bernet</t>
+  </si>
+  <si>
+    <t>VIELLA</t>
+  </si>
+  <si>
+    <t>09 77 63 23 43</t>
+  </si>
+  <si>
+    <t>DOMAINE DE BERNET Pacherenc du Vic-Bilh</t>
+  </si>
+  <si>
+    <t>DOMAINE DE BERNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    CHATEAU D'OLLIERES    </t>
+  </si>
+  <si>
+    <t>Charles ROUY</t>
+  </si>
+  <si>
+    <t>Le Château</t>
+  </si>
+  <si>
+    <t>83470</t>
+  </si>
+  <si>
+    <t>OLLIERES</t>
+  </si>
+  <si>
+    <t>04 94 59 85 57</t>
+  </si>
+  <si>
+    <t>www.chateau-ollieres.com</t>
+  </si>
+  <si>
+    <t>CHATEAU D'OLLIERES Coteaux Varois en Provence</t>
+  </si>
+  <si>
+    <t>CHATEAU D'OLLIERES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE LAOUGUÉ    </t>
+  </si>
+  <si>
+    <t>Pierre DABADIE</t>
+  </si>
+  <si>
+    <t>Route De Madiran</t>
+  </si>
+  <si>
+    <t>05 62 69 90 05</t>
+  </si>
+  <si>
+    <t>www.domaine-laougue.fr</t>
+  </si>
+  <si>
+    <t>DOMAINE LAOUGUE Madiran</t>
+  </si>
+  <si>
+    <t>A.O.C Madiran</t>
+  </si>
+  <si>
+    <t>DOMAINE LAOUGUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE ENTRAS    </t>
+  </si>
+  <si>
+    <t>Michel MAESTROJUAN</t>
+  </si>
+  <si>
+    <t>32410</t>
+  </si>
+  <si>
+    <t>AYGUETINTE</t>
+  </si>
+  <si>
+    <t>05 62 68 11 41</t>
+  </si>
+  <si>
+    <t>www.domaine-entras.com</t>
+  </si>
+  <si>
+    <t>DOMAINE DE BORDENEUVE ENTRAS Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DE BORDENEUVE ENTRAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    CHATEAU LA GORDONNE    </t>
+  </si>
+  <si>
+    <t>Nicolas JULIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE RIMAURESQ    </t>
+  </si>
+  <si>
+    <t>Pierre DUFFORT</t>
+  </si>
+  <si>
+    <t>Route De Notre Dame Des Anges</t>
+  </si>
+  <si>
+    <t>83790</t>
+  </si>
+  <si>
+    <t>PIGNANS</t>
+  </si>
+  <si>
+    <t>04 94 48 80 45</t>
+  </si>
+  <si>
+    <t>www.rimauresq.fr</t>
+  </si>
+  <si>
+    <t>DOMAINE DE RIMAURESQ Côtes de Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE DE RIMAURESQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    CHATEAU DUVIVIER    </t>
+  </si>
+  <si>
+    <t>Erik BERGMANN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE SANS    </t>
+  </si>
+  <si>
+    <t>Alain FILARTIGUE</t>
+  </si>
+  <si>
+    <t>32800</t>
+  </si>
+  <si>
+    <t>CAZENEUVE</t>
+  </si>
+  <si>
+    <t>05 62 09 77 00</t>
+  </si>
+  <si>
+    <t>DOMAINE DE SANS Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DE SANS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DU PAJOT    </t>
+  </si>
+  <si>
+    <t>Damien BARREAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    S.C. CHÂTEAU DU TARIQUET    </t>
+  </si>
+  <si>
+    <t>Famille GRASSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    MORLAN ERIC    </t>
+  </si>
+  <si>
+    <t>Eric MORLAN</t>
+  </si>
+  <si>
+    <t>Saint-Amand</t>
+  </si>
+  <si>
+    <t>EAUZE</t>
+  </si>
+  <si>
+    <t>05 62 09 89 89</t>
+  </si>
+  <si>
+    <t>DOMAINE DU MANDILLET Vin de France</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>S.I.G Vin de France</t>
+  </si>
+  <si>
+    <t>DOMAINE DU MANDILLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    VIGNOBLES FONTAN    </t>
+  </si>
+  <si>
+    <t>Nathalie GOMA</t>
+  </si>
+  <si>
+    <t>Nadège FONTAN</t>
+  </si>
+  <si>
+    <t>Maubet</t>
+  </si>
+  <si>
+    <t>NOULENS</t>
+  </si>
+  <si>
+    <t>05 62 08 55 28</t>
+  </si>
+  <si>
+    <t>www.vignoblesfontan.com</t>
+  </si>
+  <si>
+    <t>DOMAINE DE MAUBET Floc de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DE MAUBET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE SACARRON    </t>
+  </si>
+  <si>
+    <t>Michèle DECOMIS</t>
+  </si>
+  <si>
+    <t>Quartier Sacaron</t>
+  </si>
+  <si>
+    <t>83910</t>
+  </si>
+  <si>
+    <t>POURRIERES</t>
+  </si>
+  <si>
+    <t>04 94 78 58 66</t>
+  </si>
+  <si>
+    <t>DOMAINE DE SACARRON Côtes de Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE DE SACARRON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE PICARDON    </t>
+  </si>
+  <si>
+    <t>Jean-Pierre RANDE</t>
+  </si>
+  <si>
+    <t>Myriam RANDE</t>
+  </si>
+  <si>
+    <t>Picardon</t>
+  </si>
+  <si>
+    <t>REANS</t>
+  </si>
+  <si>
+    <t>05 62 09 95 52</t>
+  </si>
+  <si>
+    <t>http://domaine-picardon.jimdo.com/</t>
+  </si>
+  <si>
+    <t>DOMAINE DE PICARDON Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DE PICARDON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    G.F.A VIGNOBLES DUBOSCQ HENRI    </t>
+  </si>
+  <si>
+    <t>Henri et Fils DUBOSCQ</t>
+  </si>
+  <si>
+    <t>Monplaisir</t>
+  </si>
+  <si>
+    <t>05 56 59 30 54</t>
+  </si>
+  <si>
+    <t>DOMAINE DUBOSCQ-MONPLAISIR Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DUBOSCQ-MONPLAISIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    CHATEAU DE PERCHADE    </t>
+  </si>
+  <si>
+    <t>Marie-Laure FACCA</t>
+  </si>
+  <si>
+    <t>910 Route Des Pyrénées</t>
+  </si>
+  <si>
+    <t>40320</t>
+  </si>
+  <si>
+    <t>PAYROS - CAZAUTETS</t>
+  </si>
+  <si>
+    <t>05 58 44 50 68</t>
+  </si>
+  <si>
+    <t>www.tursan-dulucq.com</t>
+  </si>
+  <si>
+    <t>CHATEAU DE PERCHADE Tursan</t>
+  </si>
+  <si>
+    <t>A.O.C Tursan</t>
+  </si>
+  <si>
+    <t>CHATEAU DE PERCHADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    EARL DE FARON    </t>
+  </si>
+  <si>
+    <t>Christian MONTELIEU</t>
+  </si>
+  <si>
+    <t>Faron</t>
+  </si>
+  <si>
+    <t>BRETAGNE D'ARMAGNAC</t>
+  </si>
+  <si>
+    <t>05 62 09 93 84</t>
+  </si>
+  <si>
+    <t>DOMAINE DE FARON Floc de Gascogne</t>
+  </si>
+  <si>
+    <t>DOMAINE DE FARON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE LA BOUVERIE    </t>
+  </si>
+  <si>
+    <t>Jean LAPONCHE</t>
+  </si>
+  <si>
+    <t>Domaine Viticole De La Bouverie - Quartier Collet Redon</t>
+  </si>
+  <si>
+    <t>83520</t>
+  </si>
+  <si>
+    <t>ROQUEBRUNE SUR ARGENS</t>
+  </si>
+  <si>
+    <t>04 94 44 00 81</t>
+  </si>
+  <si>
+    <t>http://www.domainedelabouverie.com/</t>
+  </si>
+  <si>
+    <t>DOMAINE DE LA BOUVERIE Côtes de Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE DE LA BOUVERIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE MAS THERESE    </t>
+  </si>
+  <si>
+    <t>Aurore BLANC-GANTELME</t>
+  </si>
+  <si>
+    <t>1230, Route Des Oratoires</t>
+  </si>
+  <si>
+    <t>83330</t>
+  </si>
+  <si>
+    <t>SAINTE ANNE DU CASTELLET</t>
+  </si>
+  <si>
+    <t>04 94 35 65 18</t>
+  </si>
+  <si>
+    <t>DOMAINE MAS THERESE Bandol</t>
+  </si>
+  <si>
+    <t>A.O.C Bandol</t>
+  </si>
+  <si>
+    <t>DOMAINE MAS THERESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DES SARRINS    </t>
+  </si>
+  <si>
+    <t>Aymeric PAILLARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE LA BASTIDE DES PRES    </t>
+  </si>
+  <si>
+    <t>Franck HERAUD</t>
+  </si>
+  <si>
+    <t>Route De Mappe</t>
+  </si>
+  <si>
+    <t>SAINT ANTONIN DU VAR</t>
+  </si>
+  <si>
+    <t>04 94 04 49 04</t>
+  </si>
+  <si>
+    <t>DOMAINE LA BASTIDE DES PRES Côtes de Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE LA BASTIDE DES PRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE L'ESTAGNOL    </t>
+  </si>
+  <si>
+    <t>Sandrine FERAUD</t>
+  </si>
+  <si>
+    <t>1426, Route De La Cadière-Quartier L'Estagnol-D 66</t>
+  </si>
+  <si>
+    <t>83270</t>
+  </si>
+  <si>
+    <t>SAINT CYR SUR MER</t>
+  </si>
+  <si>
+    <t>06 01 01 35 52</t>
+  </si>
+  <si>
+    <t>DOMAINE DE L'ESTAGNOL Bandol</t>
+  </si>
+  <si>
+    <t>DOMAINE DE L'ESTAGNOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    DOMAINE DE LA FAMILLE COULOMB    </t>
+  </si>
+  <si>
+    <t>Patrick APKARIAN</t>
+  </si>
+  <si>
+    <t>280 Les Plaines De L'Aire</t>
+  </si>
+  <si>
+    <t>SEILLONS SOURCE D'ARGENS</t>
+  </si>
+  <si>
+    <t>04 94 72 50 54</t>
+  </si>
+  <si>
+    <t>DOMAINE COULOMB Coteaux Varois en Provence</t>
+  </si>
+  <si>
+    <t>DOMAINE COULOMB</t>
   </si>
 </sst>
 </file>
@@ -540,7 +1188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -991,87 +1639,87 @@
         <v>78</v>
       </c>
       <c r="B11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="C11" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="H11" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="J11" t="s" s="0">
-        <v>85</v>
-      </c>
       <c r="K11" t="s" s="0">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N11" t="s" s="0">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="K12" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="B12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="J12" t="s" s="0">
+      <c r="L12" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="K12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="L12" t="s" s="0">
-        <v>15</v>
-      </c>
       <c r="M12" t="s" s="0">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -1468,6 +2116,1326 @@
       </c>
       <c r="N21" t="s" s="0">
         <v>28</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K22" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="L22" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="M22" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N22" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K23" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L23" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="M23" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N23" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="H24" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="J24" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K24" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L24" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="M24" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="N24" t="s" s="0">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="J25" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K25" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L25" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="M25" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N25" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="H26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="J26" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K26" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="L26" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="M26" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N26" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="J27" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K27" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="L27" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="M27" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N27" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="J28" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K28" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="L28" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="M28" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="N28" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I29" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="J29" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K29" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="L29" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="M29" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="N29" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="H30" t="s" s="0">
+        <v>212</v>
+      </c>
+      <c r="I30" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="J30" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K30" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="L30" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="M30" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N30" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="J31" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K31" t="s" s="0">
+        <v>221</v>
+      </c>
+      <c r="L31" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="M31" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N31" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="F32" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="H32" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="J32" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K32" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L32" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="M32" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N32" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J33" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="K33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="L33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="N33" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>235</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="F34" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="H34" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="J34" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K34" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="L34" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="M34" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N34" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J35" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="K35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="L35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="N35" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="F36" t="s" s="0">
+        <v>247</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="H36" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="J36" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K36" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L36" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="M36" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N36" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>251</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J37" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="K37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="L37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="N37" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J38" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="K38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="L38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="N38" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="F39" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="H39" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="J39" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="K39" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="L39" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="M39" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N39" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="H40" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="I40" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="J40" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K40" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="L40" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="M40" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="N40" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>273</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>276</v>
+      </c>
+      <c r="F41" t="s" s="0">
+        <v>277</v>
+      </c>
+      <c r="G41" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="H41" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s" s="0">
+        <v>279</v>
+      </c>
+      <c r="J41" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K41" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="L41" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="M41" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N41" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>282</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="F42" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="G42" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="H42" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="I42" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="J42" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K42" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L42" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="M42" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N42" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="F43" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="G43" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="H43" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="J43" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K43" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="L43" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="M43" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N43" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="H44" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="I44" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="J44" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K44" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="L44" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="M44" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N44" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="G45" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="H45" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="J45" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K45" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="L45" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="M45" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="N45" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="G46" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="H46" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="I46" t="s" s="0">
+        <v>320</v>
+      </c>
+      <c r="J46" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K46" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="L46" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="M46" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N46" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="F47" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="G47" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="H47" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="J47" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K47" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="L47" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="M47" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N47" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>331</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="J48" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="K48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="L48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="N48" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>333</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="F49" t="s" s="0">
+        <v>336</v>
+      </c>
+      <c r="G49" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="H49" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s" s="0">
+        <v>338</v>
+      </c>
+      <c r="J49" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K49" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="L49" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="M49" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N49" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>340</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="F50" t="s" s="0">
+        <v>344</v>
+      </c>
+      <c r="G50" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="H50" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s" s="0">
+        <v>346</v>
+      </c>
+      <c r="J50" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K50" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="L50" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="M50" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N50" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="F51" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="G51" t="s" s="0">
+        <v>352</v>
+      </c>
+      <c r="H51" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s" s="0">
+        <v>353</v>
+      </c>
+      <c r="J51" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K51" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="L51" t="s" s="0">
+        <v>354</v>
+      </c>
+      <c r="M51" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="N51" t="s" s="0">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>